<commit_message>
Updated Pinouts.  50 Bands
</commit_message>
<xml_diff>
--- a/FFT-42 Band 8.2 octave 36000 sample.xlsx
+++ b/FFT-42 Band 8.2 octave 36000 sample.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="34290" yWindow="2895" windowWidth="17280" windowHeight="8970"/>
+    <workbookView xWindow="34290" yWindow="2895" windowWidth="17280" windowHeight="8970" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t>Sample Rate</t>
   </si>
@@ -109,13 +110,35 @@
   <si>
     <t>Center of highest required band. Set this to below the Nyquist frequency</t>
   </si>
+  <si>
+    <t>Total Bands</t>
+  </si>
+  <si>
+    <t>LED's per Band</t>
+  </si>
+  <si>
+    <t>Octives</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
+  </si>
+  <si>
+    <t>Top Freq</t>
+  </si>
+  <si>
+    <t>LEDs Per Octave</t>
+  </si>
+  <si>
+    <t>Total LEDs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -260,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -276,11 +299,59 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -614,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,7 +1931,7 @@
         <v>2271.006161918106</v>
       </c>
       <c r="G59" s="11">
-        <f t="shared" ref="G52:G74" si="10">F59-F58</f>
+        <f t="shared" ref="G59:G74" si="10">F59-F58</f>
         <v>293.9805493908957</v>
       </c>
     </row>
@@ -2256,20 +2327,2418 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B17:F17">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>$B$17&lt;$B$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:F45">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$B18&lt;$B$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:F74">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$B46&lt;$B$9</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L99"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17:G75"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>36000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>8.25</v>
+      </c>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="14">
+        <f>POWER(2,K5)</f>
+        <v>304.43702144069641</v>
+      </c>
+      <c r="L6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="17">
+        <f>K7</f>
+        <v>16744.036179238301</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="14">
+        <f>K6*B6</f>
+        <v>16744.036179238301</v>
+      </c>
+      <c r="L7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4096</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8">
+        <v>7</v>
+      </c>
+      <c r="L8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
+        <f>K9</f>
+        <v>58.75</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9">
+        <v>58.5</v>
+      </c>
+      <c r="K9">
+        <f>(K5*K8)+1</f>
+        <v>58.75</v>
+      </c>
+      <c r="L9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13">
+        <f>POWER(B7/B6,1/(B9-1))</f>
+        <v>1.1040895136738123</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <f>B5/2</f>
+        <v>18000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f>B5/B8</f>
+        <v>8.7890625</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <f>B8/2-1</f>
+        <v>2047</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
+        <v>0</v>
+      </c>
+      <c r="C17" s="12">
+        <f t="shared" ref="C17:C74" si="0">$B$6*POWER($B$11,B17)</f>
+        <v>55</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" ref="D17:D74" si="1">C17/$B$13</f>
+        <v>6.2577777777777781</v>
+      </c>
+      <c r="E17" s="15">
+        <v>0</v>
+      </c>
+      <c r="F17" s="16">
+        <f>((D18-D17)/2)+D17</f>
+        <v>6.5834623005616173</v>
+      </c>
+      <c r="G17" s="11">
+        <f>F17</f>
+        <v>6.5834623005616173</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
+        <f>B17+1</f>
+        <v>1</v>
+      </c>
+      <c r="C18" s="12">
+        <f t="shared" si="0"/>
+        <v>60.724923252059675</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="1"/>
+        <v>6.9091468233454565</v>
+      </c>
+      <c r="E18" s="15">
+        <f>F17</f>
+        <v>6.5834623005616173</v>
+      </c>
+      <c r="F18" s="16">
+        <f>((D19-D18)/2)+D18</f>
+        <v>7.2687316897169527</v>
+      </c>
+      <c r="G18" s="11">
+        <f t="shared" ref="G18:G81" si="2">F18</f>
+        <v>7.2687316897169527</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
+        <f t="shared" ref="B19:B83" si="3">B18+1</f>
+        <v>2</v>
+      </c>
+      <c r="C19" s="12">
+        <f t="shared" si="0"/>
+        <v>67.04575098124613</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="1"/>
+        <v>7.6283165560884489</v>
+      </c>
+      <c r="E19" s="15">
+        <f t="shared" ref="E19:E74" si="4">F18</f>
+        <v>7.2687316897169527</v>
+      </c>
+      <c r="F19" s="16">
+        <f t="shared" ref="F19:F74" si="5">((D20-D19)/2)+D19</f>
+        <v>8.0253304363250173</v>
+      </c>
+      <c r="G19" s="11">
+        <f t="shared" si="2"/>
+        <v>8.0253304363250173</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="C20" s="12">
+        <f t="shared" si="0"/>
+        <v>74.024510594779571</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="1"/>
+        <v>8.4223443165615866</v>
+      </c>
+      <c r="E20" s="15">
+        <f t="shared" si="4"/>
+        <v>8.0253304363250173</v>
+      </c>
+      <c r="F20" s="16">
+        <f t="shared" si="5"/>
+        <v>8.8606831785137317</v>
+      </c>
+      <c r="G20" s="11">
+        <f t="shared" si="2"/>
+        <v>8.8606831785137317</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="C21" s="12">
+        <f t="shared" si="0"/>
+        <v>81.729685902532125</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="1"/>
+        <v>9.2990220404658768</v>
+      </c>
+      <c r="E21" s="15">
+        <f t="shared" si="4"/>
+        <v>8.8606831785137317</v>
+      </c>
+      <c r="F21" s="16">
+        <f t="shared" si="5"/>
+        <v>9.782987381382954</v>
+      </c>
+      <c r="G21" s="11">
+        <f t="shared" si="2"/>
+        <v>9.782987381382954</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="C22" s="12">
+        <f t="shared" si="0"/>
+        <v>90.236889160840121</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="1"/>
+        <v>10.266952722300031</v>
+      </c>
+      <c r="E22" s="15">
+        <f t="shared" si="4"/>
+        <v>9.782987381382954</v>
+      </c>
+      <c r="F22" s="16">
+        <f t="shared" si="5"/>
+        <v>10.801293780188148</v>
+      </c>
+      <c r="G22" s="11">
+        <f t="shared" si="2"/>
+        <v>10.801293780188148</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="C23" s="12">
+        <f t="shared" si="0"/>
+        <v>99.62960306902967</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="1"/>
+        <v>11.335634838076265</v>
+      </c>
+      <c r="E23" s="15">
+        <f t="shared" si="4"/>
+        <v>10.801293780188148</v>
+      </c>
+      <c r="F23" s="16">
+        <f t="shared" si="5"/>
+        <v>11.925595196815905</v>
+      </c>
+      <c r="G23" s="11">
+        <f t="shared" si="2"/>
+        <v>11.925595196815905</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="C24" s="12">
+        <f t="shared" si="0"/>
+        <v>109.99999999999991</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="1"/>
+        <v>12.515555555555546</v>
+      </c>
+      <c r="E24" s="15">
+        <f t="shared" si="4"/>
+        <v>11.925595196815905</v>
+      </c>
+      <c r="F24" s="16">
+        <f t="shared" si="5"/>
+        <v>13.166924601123224</v>
+      </c>
+      <c r="G24" s="11">
+        <f t="shared" si="2"/>
+        <v>13.166924601123224</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="C25" s="12">
+        <f t="shared" si="0"/>
+        <v>121.44984650411925</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="1"/>
+        <v>13.818293646690901</v>
+      </c>
+      <c r="E25" s="15">
+        <f t="shared" si="4"/>
+        <v>13.166924601123224</v>
+      </c>
+      <c r="F25" s="16">
+        <f t="shared" si="5"/>
+        <v>14.537463379433895</v>
+      </c>
+      <c r="G25" s="11">
+        <f t="shared" si="2"/>
+        <v>14.537463379433895</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="C26" s="12">
+        <f t="shared" si="0"/>
+        <v>134.09150196249217</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="1"/>
+        <v>15.256633112176887</v>
+      </c>
+      <c r="E26" s="15">
+        <f t="shared" si="4"/>
+        <v>14.537463379433895</v>
+      </c>
+      <c r="F26" s="16">
+        <f t="shared" si="5"/>
+        <v>16.050660872650024</v>
+      </c>
+      <c r="G26" s="11">
+        <f t="shared" si="2"/>
+        <v>16.050660872650024</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="C27" s="12">
+        <f t="shared" si="0"/>
+        <v>148.049021189559</v>
+      </c>
+      <c r="D27" s="7">
+        <f t="shared" si="1"/>
+        <v>16.844688633123159</v>
+      </c>
+      <c r="E27" s="15">
+        <f t="shared" si="4"/>
+        <v>16.050660872650024</v>
+      </c>
+      <c r="F27" s="16">
+        <f t="shared" si="5"/>
+        <v>17.721366357027449</v>
+      </c>
+      <c r="G27" s="11">
+        <f t="shared" si="2"/>
+        <v>17.721366357027449</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="C28" s="12">
+        <f t="shared" si="0"/>
+        <v>163.45937180506414</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="1"/>
+        <v>18.598044080931743</v>
+      </c>
+      <c r="E28" s="15">
+        <f t="shared" si="4"/>
+        <v>17.721366357027449</v>
+      </c>
+      <c r="F28" s="16">
+        <f t="shared" si="5"/>
+        <v>19.565974762765897</v>
+      </c>
+      <c r="G28" s="11">
+        <f t="shared" si="2"/>
+        <v>19.565974762765897</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="C29" s="12">
+        <f t="shared" si="0"/>
+        <v>180.4737783216801</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="1"/>
+        <v>20.533905444600048</v>
+      </c>
+      <c r="E29" s="15">
+        <f t="shared" si="4"/>
+        <v>19.565974762765897</v>
+      </c>
+      <c r="F29" s="16">
+        <f t="shared" si="5"/>
+        <v>21.602587560376278</v>
+      </c>
+      <c r="G29" s="11">
+        <f t="shared" si="2"/>
+        <v>21.602587560376278</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="6">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="C30" s="12">
+        <f t="shared" si="0"/>
+        <v>199.25920613805917</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="1"/>
+        <v>22.671269676152509</v>
+      </c>
+      <c r="E30" s="15">
+        <f t="shared" si="4"/>
+        <v>21.602587560376278</v>
+      </c>
+      <c r="F30" s="16">
+        <f t="shared" si="5"/>
+        <v>23.851190393631789</v>
+      </c>
+      <c r="G30" s="11">
+        <f t="shared" si="2"/>
+        <v>23.851190393631789</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="C31" s="12">
+        <f t="shared" si="0"/>
+        <v>219.99999999999966</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="1"/>
+        <v>25.031111111111073</v>
+      </c>
+      <c r="E31" s="15">
+        <f t="shared" si="4"/>
+        <v>23.851190393631789</v>
+      </c>
+      <c r="F31" s="16">
+        <f t="shared" si="5"/>
+        <v>26.333849202246427</v>
+      </c>
+      <c r="G31" s="11">
+        <f t="shared" si="2"/>
+        <v>26.333849202246427</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="6">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="C32" s="12">
+        <f t="shared" si="0"/>
+        <v>242.8996930082383</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="1"/>
+        <v>27.63658729338178</v>
+      </c>
+      <c r="E32" s="15">
+        <f t="shared" si="4"/>
+        <v>26.333849202246427</v>
+      </c>
+      <c r="F32" s="16">
+        <f t="shared" si="5"/>
+        <v>29.074926758867765</v>
+      </c>
+      <c r="G32" s="11">
+        <f t="shared" si="2"/>
+        <v>29.074926758867765</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="C33" s="12">
+        <f t="shared" si="0"/>
+        <v>268.18300392498412</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" si="1"/>
+        <v>30.51326622435375</v>
+      </c>
+      <c r="E33" s="15">
+        <f t="shared" si="4"/>
+        <v>29.074926758867765</v>
+      </c>
+      <c r="F33" s="16">
+        <f t="shared" si="5"/>
+        <v>32.101321745300027</v>
+      </c>
+      <c r="G33" s="11">
+        <f t="shared" si="2"/>
+        <v>32.101321745300027</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="6">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="C34" s="12">
+        <f t="shared" si="0"/>
+        <v>296.09804237911783</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="1"/>
+        <v>33.689377266246296</v>
+      </c>
+      <c r="E34" s="15">
+        <f t="shared" si="4"/>
+        <v>32.101321745300027</v>
+      </c>
+      <c r="F34" s="16">
+        <f t="shared" si="5"/>
+        <v>35.44273271405487</v>
+      </c>
+      <c r="G34" s="11">
+        <f t="shared" si="2"/>
+        <v>35.44273271405487</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="6">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="C35" s="12">
+        <f t="shared" si="0"/>
+        <v>326.91874361012799</v>
+      </c>
+      <c r="D35" s="7">
+        <f t="shared" si="1"/>
+        <v>37.19608816186345</v>
+      </c>
+      <c r="E35" s="15">
+        <f t="shared" si="4"/>
+        <v>35.44273271405487</v>
+      </c>
+      <c r="F35" s="16">
+        <f t="shared" si="5"/>
+        <v>39.131949525531759</v>
+      </c>
+      <c r="G35" s="11">
+        <f t="shared" si="2"/>
+        <v>39.131949525531759</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="6">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="C36" s="12">
+        <f t="shared" si="0"/>
+        <v>360.94755664335997</v>
+      </c>
+      <c r="D36" s="7">
+        <f t="shared" si="1"/>
+        <v>41.067810889200068</v>
+      </c>
+      <c r="E36" s="15">
+        <f t="shared" si="4"/>
+        <v>39.131949525531759</v>
+      </c>
+      <c r="F36" s="16">
+        <f t="shared" si="5"/>
+        <v>43.205175120752529</v>
+      </c>
+      <c r="G36" s="11">
+        <f t="shared" si="2"/>
+        <v>43.205175120752529</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="C37" s="12">
+        <f t="shared" si="0"/>
+        <v>398.51841227611806</v>
+      </c>
+      <c r="D37" s="7">
+        <f t="shared" si="1"/>
+        <v>45.342539352304989</v>
+      </c>
+      <c r="E37" s="15">
+        <f t="shared" si="4"/>
+        <v>43.205175120752529</v>
+      </c>
+      <c r="F37" s="16">
+        <f t="shared" si="5"/>
+        <v>47.70238078726355</v>
+      </c>
+      <c r="G37" s="11">
+        <f t="shared" si="2"/>
+        <v>47.70238078726355</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="6">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="C38" s="12">
+        <f t="shared" si="0"/>
+        <v>439.99999999999903</v>
+      </c>
+      <c r="D38" s="7">
+        <f t="shared" si="1"/>
+        <v>50.062222222222111</v>
+      </c>
+      <c r="E38" s="15">
+        <f t="shared" si="4"/>
+        <v>47.70238078726355</v>
+      </c>
+      <c r="F38" s="16">
+        <f t="shared" si="5"/>
+        <v>52.667698404492825</v>
+      </c>
+      <c r="G38" s="11">
+        <f t="shared" si="2"/>
+        <v>52.667698404492825</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="6">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="C39" s="12">
+        <f t="shared" si="0"/>
+        <v>485.79938601647632</v>
+      </c>
+      <c r="D39" s="7">
+        <f t="shared" si="1"/>
+        <v>55.273174586763531</v>
+      </c>
+      <c r="E39" s="15">
+        <f t="shared" si="4"/>
+        <v>52.667698404492825</v>
+      </c>
+      <c r="F39" s="16">
+        <f t="shared" si="5"/>
+        <v>58.149853517735494</v>
+      </c>
+      <c r="G39" s="11">
+        <f t="shared" si="2"/>
+        <v>58.149853517735494</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="6">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="C40" s="12">
+        <f t="shared" si="0"/>
+        <v>536.3660078499679</v>
+      </c>
+      <c r="D40" s="7">
+        <f t="shared" si="1"/>
+        <v>61.026532448707457</v>
+      </c>
+      <c r="E40" s="15">
+        <f t="shared" si="4"/>
+        <v>58.149853517735494</v>
+      </c>
+      <c r="F40" s="16">
+        <f t="shared" si="5"/>
+        <v>64.202643490599996</v>
+      </c>
+      <c r="G40" s="11">
+        <f t="shared" si="2"/>
+        <v>64.202643490599996</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="6">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="C41" s="12">
+        <f t="shared" si="0"/>
+        <v>592.1960847582352</v>
+      </c>
+      <c r="D41" s="7">
+        <f t="shared" si="1"/>
+        <v>67.378754532492536</v>
+      </c>
+      <c r="E41" s="15">
+        <f t="shared" si="4"/>
+        <v>64.202643490599996</v>
+      </c>
+      <c r="F41" s="16">
+        <f t="shared" si="5"/>
+        <v>70.885465428109697</v>
+      </c>
+      <c r="G41" s="11">
+        <f t="shared" si="2"/>
+        <v>70.885465428109697</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="6">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="C42" s="12">
+        <f t="shared" si="0"/>
+        <v>653.83748722025553</v>
+      </c>
+      <c r="D42" s="7">
+        <f t="shared" si="1"/>
+        <v>74.392176323726858</v>
+      </c>
+      <c r="E42" s="15">
+        <f t="shared" si="4"/>
+        <v>70.885465428109697</v>
+      </c>
+      <c r="F42" s="16">
+        <f t="shared" si="5"/>
+        <v>78.263899051063461</v>
+      </c>
+      <c r="G42" s="11">
+        <f t="shared" si="2"/>
+        <v>78.263899051063461</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="6">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="C43" s="12">
+        <f t="shared" si="0"/>
+        <v>721.89511328671938</v>
+      </c>
+      <c r="D43" s="7">
+        <f t="shared" si="1"/>
+        <v>82.135621778400065</v>
+      </c>
+      <c r="E43" s="15">
+        <f t="shared" si="4"/>
+        <v>78.263899051063461</v>
+      </c>
+      <c r="F43" s="16">
+        <f t="shared" si="5"/>
+        <v>86.410350241504986</v>
+      </c>
+      <c r="G43" s="11">
+        <f t="shared" si="2"/>
+        <v>86.410350241504986</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="6">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="C44" s="12">
+        <f t="shared" si="0"/>
+        <v>797.03682455223554</v>
+      </c>
+      <c r="D44" s="7">
+        <f t="shared" si="1"/>
+        <v>90.685078704609907</v>
+      </c>
+      <c r="E44" s="15">
+        <f t="shared" si="4"/>
+        <v>86.410350241504986</v>
+      </c>
+      <c r="F44" s="16">
+        <f t="shared" si="5"/>
+        <v>95.404761574527029</v>
+      </c>
+      <c r="G44" s="11">
+        <f t="shared" si="2"/>
+        <v>95.404761574527029</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="6">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="C45" s="12">
+        <f t="shared" si="0"/>
+        <v>879.99999999999739</v>
+      </c>
+      <c r="D45" s="7">
+        <f t="shared" si="1"/>
+        <v>100.12444444444415</v>
+      </c>
+      <c r="E45" s="15">
+        <f t="shared" si="4"/>
+        <v>95.404761574527029</v>
+      </c>
+      <c r="F45" s="16">
+        <f t="shared" si="5"/>
+        <v>105.33539680898556</v>
+      </c>
+      <c r="G45" s="11">
+        <f t="shared" si="2"/>
+        <v>105.33539680898556</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="6">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="C46" s="12">
+        <f t="shared" si="0"/>
+        <v>971.59877203295184</v>
+      </c>
+      <c r="D46" s="7">
+        <f t="shared" si="1"/>
+        <v>110.54634917352696</v>
+      </c>
+      <c r="E46" s="15">
+        <f t="shared" si="4"/>
+        <v>105.33539680898556</v>
+      </c>
+      <c r="F46" s="16">
+        <f t="shared" si="5"/>
+        <v>116.29970703547089</v>
+      </c>
+      <c r="G46" s="11">
+        <f t="shared" si="2"/>
+        <v>116.29970703547089</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="6">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="C47" s="12">
+        <f t="shared" si="0"/>
+        <v>1072.7320156999349</v>
+      </c>
+      <c r="D47" s="7">
+        <f t="shared" si="1"/>
+        <v>122.05306489741481</v>
+      </c>
+      <c r="E47" s="15">
+        <f t="shared" si="4"/>
+        <v>116.29970703547089</v>
+      </c>
+      <c r="F47" s="16">
+        <f t="shared" si="5"/>
+        <v>128.40528698119988</v>
+      </c>
+      <c r="G47" s="11">
+        <f t="shared" si="2"/>
+        <v>128.40528698119988</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="6">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="C48" s="12">
+        <f t="shared" si="0"/>
+        <v>1184.3921695164693</v>
+      </c>
+      <c r="D48" s="7">
+        <f t="shared" si="1"/>
+        <v>134.75750906498496</v>
+      </c>
+      <c r="E48" s="15">
+        <f t="shared" si="4"/>
+        <v>128.40528698119988</v>
+      </c>
+      <c r="F48" s="16">
+        <f t="shared" si="5"/>
+        <v>141.77093085621928</v>
+      </c>
+      <c r="G48" s="11">
+        <f t="shared" si="2"/>
+        <v>141.77093085621928</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="6">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="C49" s="12">
+        <f t="shared" si="0"/>
+        <v>1307.6749744405101</v>
+      </c>
+      <c r="D49" s="7">
+        <f t="shared" si="1"/>
+        <v>148.7843526474536</v>
+      </c>
+      <c r="E49" s="15">
+        <f t="shared" si="4"/>
+        <v>141.77093085621928</v>
+      </c>
+      <c r="F49" s="16">
+        <f t="shared" si="5"/>
+        <v>156.52779810212681</v>
+      </c>
+      <c r="G49" s="11">
+        <f t="shared" si="2"/>
+        <v>156.52779810212681</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="6">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="C50" s="12">
+        <f t="shared" si="0"/>
+        <v>1443.7902265734376</v>
+      </c>
+      <c r="D50" s="7">
+        <f t="shared" si="1"/>
+        <v>164.27124355680002</v>
+      </c>
+      <c r="E50" s="15">
+        <f t="shared" si="4"/>
+        <v>156.52779810212681</v>
+      </c>
+      <c r="F50" s="16">
+        <f t="shared" si="5"/>
+        <v>172.82070048300986</v>
+      </c>
+      <c r="G50" s="11">
+        <f t="shared" si="2"/>
+        <v>172.82070048300986</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="6">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="C51" s="12">
+        <f t="shared" si="0"/>
+        <v>1594.07364910447</v>
+      </c>
+      <c r="D51" s="7">
+        <f t="shared" si="1"/>
+        <v>181.3701574092197</v>
+      </c>
+      <c r="E51" s="15">
+        <f t="shared" si="4"/>
+        <v>172.82070048300986</v>
+      </c>
+      <c r="F51" s="16">
+        <f t="shared" si="5"/>
+        <v>190.80952314905392</v>
+      </c>
+      <c r="G51" s="11">
+        <f t="shared" si="2"/>
+        <v>190.80952314905392</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="6">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="C52" s="12">
+        <f t="shared" si="0"/>
+        <v>1759.9999999999934</v>
+      </c>
+      <c r="D52" s="7">
+        <f t="shared" si="1"/>
+        <v>200.24888888888813</v>
+      </c>
+      <c r="E52" s="15">
+        <f t="shared" si="4"/>
+        <v>190.80952314905392</v>
+      </c>
+      <c r="F52" s="16">
+        <f t="shared" si="5"/>
+        <v>210.67079361797096</v>
+      </c>
+      <c r="G52" s="11">
+        <f t="shared" si="2"/>
+        <v>210.67079361797096</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="6">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="C53" s="12">
+        <f t="shared" si="0"/>
+        <v>1943.1975440659021</v>
+      </c>
+      <c r="D53" s="7">
+        <f t="shared" si="1"/>
+        <v>221.09269834705376</v>
+      </c>
+      <c r="E53" s="15">
+        <f t="shared" si="4"/>
+        <v>210.67079361797096</v>
+      </c>
+      <c r="F53" s="16">
+        <f t="shared" si="5"/>
+        <v>232.59941407094163</v>
+      </c>
+      <c r="G53" s="11">
+        <f t="shared" si="2"/>
+        <v>232.59941407094163</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="6">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="C54" s="12">
+        <f t="shared" si="0"/>
+        <v>2145.4640313998684</v>
+      </c>
+      <c r="D54" s="7">
+        <f t="shared" si="1"/>
+        <v>244.10612979482949</v>
+      </c>
+      <c r="E54" s="15">
+        <f t="shared" si="4"/>
+        <v>232.59941407094163</v>
+      </c>
+      <c r="F54" s="16">
+        <f t="shared" si="5"/>
+        <v>256.81057396239964</v>
+      </c>
+      <c r="G54" s="11">
+        <f t="shared" si="2"/>
+        <v>256.81057396239964</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="6">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="C55" s="12">
+        <f t="shared" si="0"/>
+        <v>2368.7843390329372</v>
+      </c>
+      <c r="D55" s="7">
+        <f t="shared" si="1"/>
+        <v>269.51501812996975</v>
+      </c>
+      <c r="E55" s="15">
+        <f t="shared" si="4"/>
+        <v>256.81057396239964</v>
+      </c>
+      <c r="F55" s="16">
+        <f t="shared" si="5"/>
+        <v>283.54186171243839</v>
+      </c>
+      <c r="G55" s="11">
+        <f t="shared" si="2"/>
+        <v>283.54186171243839</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="6">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="C56" s="12">
+        <f t="shared" si="0"/>
+        <v>2615.3499488810185</v>
+      </c>
+      <c r="D56" s="7">
+        <f t="shared" si="1"/>
+        <v>297.56870529490698</v>
+      </c>
+      <c r="E56" s="15">
+        <f t="shared" si="4"/>
+        <v>283.54186171243839</v>
+      </c>
+      <c r="F56" s="16">
+        <f t="shared" si="5"/>
+        <v>313.05559620425333</v>
+      </c>
+      <c r="G56" s="11">
+        <f t="shared" si="2"/>
+        <v>313.05559620425333</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="6">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="C57" s="12">
+        <f t="shared" si="0"/>
+        <v>2887.580453146873</v>
+      </c>
+      <c r="D57" s="7">
+        <f t="shared" si="1"/>
+        <v>328.54248711359975</v>
+      </c>
+      <c r="E57" s="15">
+        <f t="shared" si="4"/>
+        <v>313.05559620425333</v>
+      </c>
+      <c r="F57" s="16">
+        <f t="shared" si="5"/>
+        <v>345.64140096601943</v>
+      </c>
+      <c r="G57" s="11">
+        <f t="shared" si="2"/>
+        <v>345.64140096601943</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="6">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="C58" s="12">
+        <f t="shared" si="0"/>
+        <v>3188.1472982089376</v>
+      </c>
+      <c r="D58" s="7">
+        <f t="shared" si="1"/>
+        <v>362.74031481843912</v>
+      </c>
+      <c r="E58" s="15">
+        <f t="shared" si="4"/>
+        <v>345.64140096601943</v>
+      </c>
+      <c r="F58" s="16">
+        <f t="shared" si="5"/>
+        <v>381.61904629810755</v>
+      </c>
+      <c r="G58" s="11">
+        <f t="shared" si="2"/>
+        <v>381.61904629810755</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="6">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="C59" s="12">
+        <f t="shared" si="0"/>
+        <v>3519.9999999999841</v>
+      </c>
+      <c r="D59" s="7">
+        <f t="shared" si="1"/>
+        <v>400.49777777777598</v>
+      </c>
+      <c r="E59" s="15">
+        <f t="shared" si="4"/>
+        <v>381.61904629810755</v>
+      </c>
+      <c r="F59" s="16">
+        <f t="shared" si="5"/>
+        <v>421.34158723594157</v>
+      </c>
+      <c r="G59" s="11">
+        <f t="shared" si="2"/>
+        <v>421.34158723594157</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="6">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="C60" s="12">
+        <f t="shared" si="0"/>
+        <v>3886.395088131801</v>
+      </c>
+      <c r="D60" s="7">
+        <f t="shared" si="1"/>
+        <v>442.18539669410711</v>
+      </c>
+      <c r="E60" s="15">
+        <f t="shared" si="4"/>
+        <v>421.34158723594157</v>
+      </c>
+      <c r="F60" s="16">
+        <f t="shared" si="5"/>
+        <v>465.19882814188281</v>
+      </c>
+      <c r="G60" s="11">
+        <f t="shared" si="2"/>
+        <v>465.19882814188281</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="6">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="C61" s="12">
+        <f t="shared" si="0"/>
+        <v>4290.9280627997332</v>
+      </c>
+      <c r="D61" s="7">
+        <f t="shared" si="1"/>
+        <v>488.21225958965852</v>
+      </c>
+      <c r="E61" s="15">
+        <f t="shared" si="4"/>
+        <v>465.19882814188281</v>
+      </c>
+      <c r="F61" s="16">
+        <f t="shared" si="5"/>
+        <v>513.62114792479883</v>
+      </c>
+      <c r="G61" s="11">
+        <f t="shared" si="2"/>
+        <v>513.62114792479883</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="6">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="C62" s="12">
+        <f t="shared" si="0"/>
+        <v>4737.5686780658707</v>
+      </c>
+      <c r="D62" s="7">
+        <f t="shared" si="1"/>
+        <v>539.03003625993904</v>
+      </c>
+      <c r="E62" s="15">
+        <f t="shared" si="4"/>
+        <v>513.62114792479883</v>
+      </c>
+      <c r="F62" s="16">
+        <f t="shared" si="5"/>
+        <v>567.08372342487633</v>
+      </c>
+      <c r="G62" s="11">
+        <f t="shared" si="2"/>
+        <v>567.08372342487633</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="6">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="C63" s="12">
+        <f t="shared" si="0"/>
+        <v>5230.6998977620324</v>
+      </c>
+      <c r="D63" s="7">
+        <f t="shared" si="1"/>
+        <v>595.1374105898135</v>
+      </c>
+      <c r="E63" s="15">
+        <f t="shared" si="4"/>
+        <v>567.08372342487633</v>
+      </c>
+      <c r="F63" s="16">
+        <f t="shared" si="5"/>
+        <v>626.11119240850621</v>
+      </c>
+      <c r="G63" s="11">
+        <f t="shared" si="2"/>
+        <v>626.11119240850621</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="6">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="C64" s="12">
+        <f t="shared" si="0"/>
+        <v>5775.1609062937414</v>
+      </c>
+      <c r="D64" s="7">
+        <f t="shared" si="1"/>
+        <v>657.08497422719904</v>
+      </c>
+      <c r="E64" s="15">
+        <f t="shared" si="4"/>
+        <v>626.11119240850621</v>
+      </c>
+      <c r="F64" s="16">
+        <f t="shared" si="5"/>
+        <v>691.28280193203841</v>
+      </c>
+      <c r="G64" s="11">
+        <f t="shared" si="2"/>
+        <v>691.28280193203841</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="6">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="C65" s="12">
+        <f t="shared" si="0"/>
+        <v>6376.2945964178707</v>
+      </c>
+      <c r="D65" s="7">
+        <f t="shared" si="1"/>
+        <v>725.48062963687778</v>
+      </c>
+      <c r="E65" s="15">
+        <f t="shared" si="4"/>
+        <v>691.28280193203841</v>
+      </c>
+      <c r="F65" s="16">
+        <f t="shared" si="5"/>
+        <v>763.23809259621453</v>
+      </c>
+      <c r="G65" s="11">
+        <f t="shared" si="2"/>
+        <v>763.23809259621453</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="6">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="C66" s="12">
+        <f t="shared" si="0"/>
+        <v>7039.9999999999636</v>
+      </c>
+      <c r="D66" s="7">
+        <f t="shared" si="1"/>
+        <v>800.99555555555139</v>
+      </c>
+      <c r="E66" s="15">
+        <f t="shared" si="4"/>
+        <v>763.23809259621453</v>
+      </c>
+      <c r="F66" s="16">
+        <f t="shared" si="5"/>
+        <v>842.68317447188258</v>
+      </c>
+      <c r="G66" s="11">
+        <f t="shared" si="2"/>
+        <v>842.68317447188258</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="6">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="C67" s="12">
+        <f t="shared" si="0"/>
+        <v>7772.7901762635975</v>
+      </c>
+      <c r="D67" s="7">
+        <f t="shared" si="1"/>
+        <v>884.37079338821377</v>
+      </c>
+      <c r="E67" s="15">
+        <f t="shared" si="4"/>
+        <v>842.68317447188258</v>
+      </c>
+      <c r="F67" s="16">
+        <f t="shared" si="5"/>
+        <v>930.39765628376495</v>
+      </c>
+      <c r="G67" s="11">
+        <f t="shared" si="2"/>
+        <v>930.39765628376495</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="6">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="C68" s="12">
+        <f t="shared" si="0"/>
+        <v>8581.8561255994591</v>
+      </c>
+      <c r="D68" s="7">
+        <f t="shared" si="1"/>
+        <v>976.42451917931623</v>
+      </c>
+      <c r="E68" s="15">
+        <f t="shared" si="4"/>
+        <v>930.39765628376495</v>
+      </c>
+      <c r="F68" s="16">
+        <f t="shared" si="5"/>
+        <v>1027.2422958495968</v>
+      </c>
+      <c r="G68" s="11">
+        <f t="shared" si="2"/>
+        <v>1027.2422958495968</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="6">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="C69" s="12">
+        <f t="shared" si="0"/>
+        <v>9475.1373561317341</v>
+      </c>
+      <c r="D69" s="7">
+        <f t="shared" si="1"/>
+        <v>1078.0600725198774</v>
+      </c>
+      <c r="E69" s="15">
+        <f t="shared" si="4"/>
+        <v>1027.2422958495968</v>
+      </c>
+      <c r="F69" s="16">
+        <f t="shared" si="5"/>
+        <v>1134.1674468497517</v>
+      </c>
+      <c r="G69" s="11">
+        <f t="shared" si="2"/>
+        <v>1134.1674468497517</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="6">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="C70" s="12">
+        <f t="shared" si="0"/>
+        <v>10461.399795524057</v>
+      </c>
+      <c r="D70" s="7">
+        <f t="shared" si="1"/>
+        <v>1190.2748211796261</v>
+      </c>
+      <c r="E70" s="15">
+        <f t="shared" si="4"/>
+        <v>1134.1674468497517</v>
+      </c>
+      <c r="F70" s="16">
+        <f t="shared" si="5"/>
+        <v>1252.2223848170115</v>
+      </c>
+      <c r="G70" s="11">
+        <f t="shared" si="2"/>
+        <v>1252.2223848170115</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="6">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="C71" s="12">
+        <f t="shared" si="0"/>
+        <v>11550.321812587476</v>
+      </c>
+      <c r="D71" s="7">
+        <f t="shared" si="1"/>
+        <v>1314.1699484543972</v>
+      </c>
+      <c r="E71" s="15">
+        <f t="shared" si="4"/>
+        <v>1252.2223848170115</v>
+      </c>
+      <c r="F71" s="16">
+        <f t="shared" si="5"/>
+        <v>1382.5656038640759</v>
+      </c>
+      <c r="G71" s="11">
+        <f t="shared" si="2"/>
+        <v>1382.5656038640759</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="6">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="C72" s="12">
+        <f t="shared" si="0"/>
+        <v>12752.589192835732</v>
+      </c>
+      <c r="D72" s="7">
+        <f t="shared" si="1"/>
+        <v>1450.9612592737544</v>
+      </c>
+      <c r="E72" s="15">
+        <f t="shared" si="4"/>
+        <v>1382.5656038640759</v>
+      </c>
+      <c r="F72" s="16">
+        <f t="shared" si="5"/>
+        <v>1526.4761851924279</v>
+      </c>
+      <c r="G72" s="11">
+        <f t="shared" si="2"/>
+        <v>1526.4761851924279</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="6">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="C73" s="12">
+        <f t="shared" si="0"/>
+        <v>14079.999999999915</v>
+      </c>
+      <c r="D73" s="7">
+        <f t="shared" si="1"/>
+        <v>1601.9911111111014</v>
+      </c>
+      <c r="E73" s="15">
+        <f t="shared" si="4"/>
+        <v>1526.4761851924279</v>
+      </c>
+      <c r="F73" s="16">
+        <f t="shared" si="5"/>
+        <v>1685.3663489437638</v>
+      </c>
+      <c r="G73" s="11">
+        <f t="shared" si="2"/>
+        <v>1685.3663489437638</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="6">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+      <c r="C74" s="12">
+        <f t="shared" si="0"/>
+        <v>15545.580352527182</v>
+      </c>
+      <c r="D74" s="7">
+        <f t="shared" si="1"/>
+        <v>1768.7415867764262</v>
+      </c>
+      <c r="E74" s="15">
+        <f t="shared" si="4"/>
+        <v>1685.3663489437638</v>
+      </c>
+      <c r="F74" s="16">
+        <f t="shared" si="5"/>
+        <v>1860.7953125675288</v>
+      </c>
+      <c r="G74" s="11">
+        <f t="shared" si="2"/>
+        <v>1860.7953125675288</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="6">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="C75" s="12">
+        <f t="shared" ref="C75:C80" si="6">$B$6*POWER($B$11,B75)</f>
+        <v>17163.712251198907</v>
+      </c>
+      <c r="D75" s="7">
+        <f t="shared" ref="D75:D80" si="7">C75/$B$13</f>
+        <v>1952.8490383586313</v>
+      </c>
+      <c r="E75" s="15">
+        <f t="shared" ref="E75:E80" si="8">F74</f>
+        <v>1860.7953125675288</v>
+      </c>
+      <c r="F75" s="16">
+        <f t="shared" ref="F75:F80" si="9">((D76-D75)/2)+D75</f>
+        <v>2054.4845916991922</v>
+      </c>
+      <c r="G75" s="11">
+        <f t="shared" si="2"/>
+        <v>2054.4845916991922</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" s="6">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="C76" s="12">
+        <f t="shared" si="6"/>
+        <v>18950.274712263454</v>
+      </c>
+      <c r="D76" s="7">
+        <f t="shared" si="7"/>
+        <v>2156.120145039753</v>
+      </c>
+      <c r="E76" s="15">
+        <f t="shared" si="8"/>
+        <v>2054.4845916991922</v>
+      </c>
+      <c r="F76" s="16">
+        <f t="shared" si="9"/>
+        <v>2268.3348936995017</v>
+      </c>
+      <c r="G76" s="11">
+        <f t="shared" si="2"/>
+        <v>2268.3348936995017</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" s="6">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="C77" s="12">
+        <f t="shared" si="6"/>
+        <v>20922.7995910481</v>
+      </c>
+      <c r="D77" s="7">
+        <f t="shared" si="7"/>
+        <v>2380.5496423592504</v>
+      </c>
+      <c r="E77" s="15">
+        <f t="shared" si="8"/>
+        <v>2268.3348936995017</v>
+      </c>
+      <c r="F77" s="16">
+        <f t="shared" si="9"/>
+        <v>2504.4447696340212</v>
+      </c>
+      <c r="G77" s="11">
+        <f t="shared" si="2"/>
+        <v>2504.4447696340212</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="6">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="C78" s="12">
+        <f t="shared" si="6"/>
+        <v>23100.643625174933</v>
+      </c>
+      <c r="D78" s="7">
+        <f t="shared" si="7"/>
+        <v>2628.3398969087925</v>
+      </c>
+      <c r="E78" s="15">
+        <f t="shared" si="8"/>
+        <v>2504.4447696340212</v>
+      </c>
+      <c r="F78" s="16">
+        <f t="shared" si="9"/>
+        <v>2765.1312077281491</v>
+      </c>
+      <c r="G78" s="11">
+        <f t="shared" si="2"/>
+        <v>2765.1312077281491</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="6">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="C79" s="12">
+        <f t="shared" si="6"/>
+        <v>25505.178385671439</v>
+      </c>
+      <c r="D79" s="7">
+        <f t="shared" si="7"/>
+        <v>2901.9225185475061</v>
+      </c>
+      <c r="E79" s="15">
+        <f t="shared" si="8"/>
+        <v>2765.1312077281491</v>
+      </c>
+      <c r="F79" s="16">
+        <f t="shared" si="9"/>
+        <v>3052.9523703848531</v>
+      </c>
+      <c r="G79" s="11">
+        <f t="shared" si="2"/>
+        <v>3052.9523703848531</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="6">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="C80" s="12">
+        <f t="shared" si="6"/>
+        <v>28159.999999999807</v>
+      </c>
+      <c r="D80" s="7">
+        <f t="shared" si="7"/>
+        <v>3203.9822222222001</v>
+      </c>
+      <c r="E80" s="15">
+        <f t="shared" si="8"/>
+        <v>3052.9523703848531</v>
+      </c>
+      <c r="F80" s="16">
+        <f t="shared" si="9"/>
+        <v>3370.7326978875244</v>
+      </c>
+      <c r="G80" s="11">
+        <f t="shared" si="2"/>
+        <v>3370.7326978875244</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="6">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="C81" s="12">
+        <f t="shared" ref="C81:C82" si="10">$B$6*POWER($B$11,B81)</f>
+        <v>31091.160705054339</v>
+      </c>
+      <c r="D81" s="7">
+        <f t="shared" ref="D81:D82" si="11">C81/$B$13</f>
+        <v>3537.4831735528492</v>
+      </c>
+      <c r="E81" s="15">
+        <f t="shared" ref="E81:E82" si="12">F80</f>
+        <v>3370.7326978875244</v>
+      </c>
+      <c r="F81" s="16">
+        <f t="shared" ref="F81:F82" si="13">((D82-D81)/2)+D81</f>
+        <v>3721.5906251350543</v>
+      </c>
+      <c r="G81" s="11">
+        <f t="shared" si="2"/>
+        <v>3721.5906251350543</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="6">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="C82" s="12">
+        <f t="shared" si="10"/>
+        <v>34327.424502397786</v>
+      </c>
+      <c r="D82" s="7">
+        <f t="shared" si="11"/>
+        <v>3905.698076717259</v>
+      </c>
+      <c r="E82" s="15">
+        <f t="shared" si="12"/>
+        <v>3721.5906251350543</v>
+      </c>
+      <c r="F82" s="16">
+        <f t="shared" si="13"/>
+        <v>4108.9691833983807</v>
+      </c>
+      <c r="G82" s="11">
+        <f t="shared" ref="G82:G99" si="14">F82</f>
+        <v>4108.9691833983807</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="6">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="C83" s="12">
+        <f t="shared" ref="C83:C99" si="15">$B$6*POWER($B$11,B83)</f>
+        <v>37900.549424526878</v>
+      </c>
+      <c r="D83" s="7">
+        <f t="shared" ref="D83:D99" si="16">C83/$B$13</f>
+        <v>4312.2402900795023</v>
+      </c>
+      <c r="E83" s="15">
+        <f t="shared" ref="E83:E99" si="17">F82</f>
+        <v>4108.9691833983807</v>
+      </c>
+      <c r="F83" s="16">
+        <f t="shared" ref="F83:F99" si="18">((D84-D83)/2)+D83</f>
+        <v>4536.6697873989997</v>
+      </c>
+      <c r="G83" s="11">
+        <f t="shared" si="14"/>
+        <v>4536.6697873989997</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="6">
+        <f t="shared" ref="B84:B99" si="19">B83+1</f>
+        <v>67</v>
+      </c>
+      <c r="C84" s="12">
+        <f t="shared" si="15"/>
+        <v>41845.599182096164</v>
+      </c>
+      <c r="D84" s="7">
+        <f t="shared" si="16"/>
+        <v>4761.0992847184971</v>
+      </c>
+      <c r="E84" s="15">
+        <f t="shared" si="17"/>
+        <v>4536.6697873989997</v>
+      </c>
+      <c r="F84" s="16">
+        <f t="shared" si="18"/>
+        <v>5008.8895392680388</v>
+      </c>
+      <c r="G84" s="11">
+        <f t="shared" si="14"/>
+        <v>5008.8895392680388</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="6">
+        <f t="shared" si="19"/>
+        <v>68</v>
+      </c>
+      <c r="C85" s="12">
+        <f t="shared" si="15"/>
+        <v>46201.287250349829</v>
+      </c>
+      <c r="D85" s="7">
+        <f t="shared" si="16"/>
+        <v>5256.6797938175805</v>
+      </c>
+      <c r="E85" s="15">
+        <f t="shared" si="17"/>
+        <v>5008.8895392680388</v>
+      </c>
+      <c r="F85" s="16">
+        <f t="shared" si="18"/>
+        <v>5530.2624154562945</v>
+      </c>
+      <c r="G85" s="11">
+        <f t="shared" si="14"/>
+        <v>5530.2624154562945</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="6">
+        <f t="shared" si="19"/>
+        <v>69</v>
+      </c>
+      <c r="C86" s="12">
+        <f t="shared" si="15"/>
+        <v>51010.356771342842</v>
+      </c>
+      <c r="D86" s="7">
+        <f t="shared" si="16"/>
+        <v>5803.8450370950077</v>
+      </c>
+      <c r="E86" s="15">
+        <f t="shared" si="17"/>
+        <v>5530.2624154562945</v>
+      </c>
+      <c r="F86" s="16">
+        <f t="shared" si="18"/>
+        <v>6105.9047407697017</v>
+      </c>
+      <c r="G86" s="11">
+        <f t="shared" si="14"/>
+        <v>6105.9047407697017</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="6">
+        <f t="shared" si="19"/>
+        <v>70</v>
+      </c>
+      <c r="C87" s="12">
+        <f t="shared" si="15"/>
+        <v>56319.999999999571</v>
+      </c>
+      <c r="D87" s="7">
+        <f t="shared" si="16"/>
+        <v>6407.9644444443957</v>
+      </c>
+      <c r="E87" s="15">
+        <f t="shared" si="17"/>
+        <v>6105.9047407697017</v>
+      </c>
+      <c r="F87" s="16">
+        <f t="shared" si="18"/>
+        <v>6741.4653957750452</v>
+      </c>
+      <c r="G87" s="11">
+        <f t="shared" si="14"/>
+        <v>6741.4653957750452</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="6">
+        <f t="shared" si="19"/>
+        <v>71</v>
+      </c>
+      <c r="C88" s="12">
+        <f t="shared" si="15"/>
+        <v>62182.321410108634</v>
+      </c>
+      <c r="D88" s="7">
+        <f t="shared" si="16"/>
+        <v>7074.9663471056938</v>
+      </c>
+      <c r="E88" s="15">
+        <f t="shared" si="17"/>
+        <v>6741.4653957750452</v>
+      </c>
+      <c r="F88" s="16">
+        <f t="shared" si="18"/>
+        <v>7443.1812502701032</v>
+      </c>
+      <c r="G88" s="11">
+        <f t="shared" si="14"/>
+        <v>7443.1812502701032</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="6">
+        <f t="shared" si="19"/>
+        <v>72</v>
+      </c>
+      <c r="C89" s="12">
+        <f t="shared" si="15"/>
+        <v>68654.849004795513</v>
+      </c>
+      <c r="D89" s="7">
+        <f t="shared" si="16"/>
+        <v>7811.3961534345117</v>
+      </c>
+      <c r="E89" s="15">
+        <f t="shared" si="17"/>
+        <v>7443.1812502701032</v>
+      </c>
+      <c r="F89" s="16">
+        <f t="shared" si="18"/>
+        <v>8217.9383667967559</v>
+      </c>
+      <c r="G89" s="11">
+        <f t="shared" si="14"/>
+        <v>8217.9383667967559</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="6">
+        <f t="shared" si="19"/>
+        <v>73</v>
+      </c>
+      <c r="C90" s="12">
+        <f t="shared" si="15"/>
+        <v>75801.098849053698</v>
+      </c>
+      <c r="D90" s="7">
+        <f t="shared" si="16"/>
+        <v>8624.4805801589991</v>
+      </c>
+      <c r="E90" s="15">
+        <f t="shared" si="17"/>
+        <v>8217.9383667967559</v>
+      </c>
+      <c r="F90" s="16">
+        <f t="shared" si="18"/>
+        <v>9073.3395747979921</v>
+      </c>
+      <c r="G90" s="11">
+        <f t="shared" si="14"/>
+        <v>9073.3395747979921</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="6">
+        <f t="shared" si="19"/>
+        <v>74</v>
+      </c>
+      <c r="C91" s="12">
+        <f t="shared" si="15"/>
+        <v>83691.198364192256</v>
+      </c>
+      <c r="D91" s="7">
+        <f t="shared" si="16"/>
+        <v>9522.1985694369851</v>
+      </c>
+      <c r="E91" s="15">
+        <f t="shared" si="17"/>
+        <v>9073.3395747979921</v>
+      </c>
+      <c r="F91" s="16">
+        <f t="shared" si="18"/>
+        <v>10017.77907853607</v>
+      </c>
+      <c r="G91" s="11">
+        <f t="shared" si="14"/>
+        <v>10017.77907853607</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="6">
+        <f t="shared" si="19"/>
+        <v>75</v>
+      </c>
+      <c r="C92" s="12">
+        <f t="shared" si="15"/>
+        <v>92402.574500699586</v>
+      </c>
+      <c r="D92" s="7">
+        <f t="shared" si="16"/>
+        <v>10513.359587635154</v>
+      </c>
+      <c r="E92" s="15">
+        <f t="shared" si="17"/>
+        <v>10017.77907853607</v>
+      </c>
+      <c r="F92" s="16">
+        <f t="shared" si="18"/>
+        <v>11060.52483091258</v>
+      </c>
+      <c r="G92" s="11">
+        <f t="shared" si="14"/>
+        <v>11060.52483091258</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="6">
+        <f t="shared" si="19"/>
+        <v>76</v>
+      </c>
+      <c r="C93" s="12">
+        <f t="shared" si="15"/>
+        <v>102020.7135426856</v>
+      </c>
+      <c r="D93" s="7">
+        <f t="shared" si="16"/>
+        <v>11607.690074190006</v>
+      </c>
+      <c r="E93" s="15">
+        <f t="shared" si="17"/>
+        <v>11060.52483091258</v>
+      </c>
+      <c r="F93" s="16">
+        <f t="shared" si="18"/>
+        <v>12211.809481539394</v>
+      </c>
+      <c r="G93" s="11">
+        <f t="shared" si="14"/>
+        <v>12211.809481539394</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="6">
+        <f t="shared" si="19"/>
+        <v>77</v>
+      </c>
+      <c r="C94" s="12">
+        <f t="shared" si="15"/>
+        <v>112639.99999999907</v>
+      </c>
+      <c r="D94" s="7">
+        <f t="shared" si="16"/>
+        <v>12815.928888888782</v>
+      </c>
+      <c r="E94" s="15">
+        <f t="shared" si="17"/>
+        <v>12211.809481539394</v>
+      </c>
+      <c r="F94" s="16">
+        <f t="shared" si="18"/>
+        <v>13482.930791550079</v>
+      </c>
+      <c r="G94" s="11">
+        <f t="shared" si="14"/>
+        <v>13482.930791550079</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="6">
+        <f t="shared" si="19"/>
+        <v>78</v>
+      </c>
+      <c r="C95" s="12">
+        <f t="shared" si="15"/>
+        <v>124364.64282021717</v>
+      </c>
+      <c r="D95" s="7">
+        <f t="shared" si="16"/>
+        <v>14149.932694211375</v>
+      </c>
+      <c r="E95" s="15">
+        <f t="shared" si="17"/>
+        <v>13482.930791550079</v>
+      </c>
+      <c r="F95" s="16">
+        <f t="shared" si="18"/>
+        <v>14886.362500540195</v>
+      </c>
+      <c r="G95" s="11">
+        <f t="shared" si="14"/>
+        <v>14886.362500540195</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="6">
+        <f t="shared" si="19"/>
+        <v>79</v>
+      </c>
+      <c r="C96" s="12">
+        <f t="shared" si="15"/>
+        <v>137309.69800959094</v>
+      </c>
+      <c r="D96" s="7">
+        <f t="shared" si="16"/>
+        <v>15622.792306869014</v>
+      </c>
+      <c r="E96" s="15">
+        <f t="shared" si="17"/>
+        <v>14886.362500540195</v>
+      </c>
+      <c r="F96" s="16">
+        <f t="shared" si="18"/>
+        <v>16435.876733593501</v>
+      </c>
+      <c r="G96" s="11">
+        <f t="shared" si="14"/>
+        <v>16435.876733593501</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" s="6">
+        <f t="shared" si="19"/>
+        <v>80</v>
+      </c>
+      <c r="C97" s="12">
+        <f t="shared" si="15"/>
+        <v>151602.19769810731</v>
+      </c>
+      <c r="D97" s="7">
+        <f t="shared" si="16"/>
+        <v>17248.961160317987</v>
+      </c>
+      <c r="E97" s="15">
+        <f t="shared" si="17"/>
+        <v>16435.876733593501</v>
+      </c>
+      <c r="F97" s="16">
+        <f t="shared" si="18"/>
+        <v>18146.679149595977</v>
+      </c>
+      <c r="G97" s="11">
+        <f t="shared" si="14"/>
+        <v>18146.679149595977</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" s="6">
+        <f t="shared" si="19"/>
+        <v>81</v>
+      </c>
+      <c r="C98" s="12">
+        <f t="shared" si="15"/>
+        <v>167382.39672838442</v>
+      </c>
+      <c r="D98" s="7">
+        <f t="shared" si="16"/>
+        <v>19044.397138873963</v>
+      </c>
+      <c r="E98" s="15">
+        <f t="shared" si="17"/>
+        <v>18146.679149595977</v>
+      </c>
+      <c r="F98" s="16">
+        <f t="shared" si="18"/>
+        <v>20035.558157072126</v>
+      </c>
+      <c r="G98" s="11">
+        <f t="shared" si="14"/>
+        <v>20035.558157072126</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B99" s="6">
+        <f t="shared" si="19"/>
+        <v>82</v>
+      </c>
+      <c r="C99" s="12">
+        <f t="shared" si="15"/>
+        <v>184805.14900139903</v>
+      </c>
+      <c r="D99" s="7">
+        <f t="shared" si="16"/>
+        <v>21026.719175270289</v>
+      </c>
+      <c r="E99" s="15">
+        <f t="shared" si="17"/>
+        <v>20035.558157072126</v>
+      </c>
+      <c r="F99" s="16">
+        <f t="shared" si="18"/>
+        <v>10513.359587635145</v>
+      </c>
+      <c r="G99" s="11">
+        <f t="shared" si="14"/>
+        <v>10513.359587635145</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B17:F17">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>$B$17&lt;$B$9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:F45">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>$B18&lt;$B$9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46:F74">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$B46&lt;$B$9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B75:F80">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$B75&lt;$B$9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:F99">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$B83&lt;$B$9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B81:F82">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$B81&lt;$B$9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>